<commit_message>
Code: feature selection 2
</commit_message>
<xml_diff>
--- a/LCDataDictionary.xlsx
+++ b/LCDataDictionary.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28810"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjoshi/Documents/LendingClub/Quarterly_Loan_Stats/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jpinzon/OneDrive/Courses/01_MLND_UDACITY/machine-learning-master/projects/06 capstone/problem_loan/Problem_loan_prediction/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22620" activeTab="1"/>
+    <workbookView xWindow="680" yWindow="460" windowWidth="24900" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" r:id="rId1"/>
@@ -2256,9 +2256,9 @@
   </sheetPr>
   <dimension ref="A1:K154"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A145" sqref="A145:B145"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A145" sqref="A145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2395,292 +2395,292 @@
       <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>54</v>
+      <c r="A15" s="9" t="s">
+        <v>345</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>337</v>
       </c>
       <c r="C15" s="24"/>
     </row>
     <row r="16" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>298</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>55</v>
+        <v>346</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>338</v>
       </c>
       <c r="C16" s="24"/>
     </row>
     <row r="17" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>56</v>
+      <c r="A17" s="9" t="s">
+        <v>351</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>371</v>
       </c>
       <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3" s="4" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>242</v>
+        <v>54</v>
       </c>
       <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>256</v>
+      <c r="A19" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>249</v>
+        <v>17</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>58</v>
+      <c r="A21" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>382</v>
       </c>
       <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>167</v>
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>242</v>
       </c>
       <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>260</v>
+        <v>255</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>256</v>
       </c>
       <c r="C23" s="5"/>
     </row>
     <row r="24" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="7" t="s">
-        <v>24</v>
+      <c r="A24" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="C24" s="5"/>
     </row>
     <row r="25" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>220</v>
+        <v>10</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>4</v>
+        <v>166</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>221</v>
+        <v>167</v>
       </c>
       <c r="C26" s="5"/>
     </row>
     <row r="27" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>60</v>
+      <c r="A27" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>260</v>
       </c>
       <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>309</v>
+      <c r="A28" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>261</v>
       </c>
       <c r="C28" s="5"/>
     </row>
     <row r="29" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>62</v>
+        <v>220</v>
       </c>
       <c r="C29" s="24"/>
     </row>
     <row r="30" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="9" t="s">
-        <v>277</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>278</v>
+      <c r="A30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>221</v>
       </c>
       <c r="C30" s="24"/>
     </row>
     <row r="31" spans="1:3" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C31" s="5"/>
     </row>
     <row r="32" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>287</v>
+        <v>352</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>288</v>
+        <v>372</v>
       </c>
       <c r="C32" s="5"/>
     </row>
     <row r="33" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
-        <v>289</v>
+        <v>357</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>290</v>
+        <v>377</v>
       </c>
       <c r="C33" s="5"/>
     </row>
     <row r="34" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>262</v>
+      <c r="A34" s="9" t="s">
+        <v>354</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>374</v>
       </c>
       <c r="C34" s="5"/>
     </row>
     <row r="35" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>64</v>
+      <c r="A35" s="9" t="s">
+        <v>347</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>367</v>
       </c>
       <c r="C35" s="5"/>
     </row>
     <row r="36" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>87</v>
+      <c r="A36" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>381</v>
       </c>
       <c r="C36" s="5"/>
     </row>
     <row r="37" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>248</v>
+      <c r="A37" s="9" t="s">
+        <v>356</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>376</v>
       </c>
       <c r="C37" s="5"/>
       <c r="I37" s="10"/>
       <c r="J37" s="11"/>
     </row>
     <row r="38" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>251</v>
+      <c r="A38" s="9" t="s">
+        <v>358</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>378</v>
       </c>
       <c r="C38" s="5"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A39" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>263</v>
+      <c r="A39" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>380</v>
       </c>
       <c r="D39" s="4"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A40" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>264</v>
+      <c r="A40" s="9" t="s">
+        <v>349</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>369</v>
       </c>
       <c r="D40" s="4"/>
     </row>
     <row r="41" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>97</v>
+      <c r="A41" s="9" t="s">
+        <v>353</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>373</v>
       </c>
       <c r="D41" s="4"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>250</v>
+      <c r="A42" s="9" t="s">
+        <v>350</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>370</v>
       </c>
       <c r="D42" s="4"/>
     </row>
     <row r="43" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>66</v>
+      <c r="A43" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>368</v>
       </c>
       <c r="D43" s="4"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>88</v>
+        <v>11</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>309</v>
       </c>
       <c r="D44" s="4"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A45" s="9" t="s">
-        <v>283</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>284</v>
+      <c r="A45" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="D45" s="4"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>67</v>
+      <c r="A46" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>278</v>
       </c>
       <c r="D46" s="4"/>
       <c r="I46" s="10"/>
@@ -2688,11 +2688,11 @@
       <c r="K46" s="11"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A47" s="9" t="s">
-        <v>299</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>132</v>
+      <c r="A47" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="D47" s="4"/>
       <c r="I47" s="10"/>
@@ -2701,10 +2701,10 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>133</v>
+        <v>287</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>288</v>
       </c>
       <c r="D48" s="4"/>
       <c r="I48" s="12"/>
@@ -2713,617 +2713,617 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>134</v>
+        <v>289</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>290</v>
       </c>
       <c r="D49" s="4"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>135</v>
+      <c r="A50" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>262</v>
       </c>
       <c r="D50" s="4"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="9" t="s">
-        <v>300</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>68</v>
+      <c r="A51" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="D51" s="4"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>69</v>
+        <v>6</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="D52" s="4"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="B53" s="9" t="s">
-        <v>136</v>
+      <c r="A53" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>248</v>
       </c>
       <c r="D53" s="4"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>70</v>
+        <v>251</v>
       </c>
       <c r="D54" s="4"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="9" t="s">
-        <v>273</v>
-      </c>
-      <c r="B55" s="9" t="s">
-        <v>274</v>
+      <c r="A55" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>263</v>
       </c>
       <c r="D55" s="4"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>72</v>
+      <c r="A56" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>264</v>
       </c>
       <c r="D56" s="4"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>303</v>
+      <c r="A57" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="D57" s="4"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="9" t="s">
-        <v>304</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>71</v>
+      <c r="A58" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>250</v>
       </c>
       <c r="D58" s="4"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="9" t="s">
-        <v>305</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>74</v>
+      <c r="A59" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="D59" s="4"/>
     </row>
     <row r="60" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>98</v>
+        <v>14</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="D60" s="4"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>137</v>
+        <v>283</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>284</v>
       </c>
       <c r="D61" s="4"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>142</v>
+      <c r="A62" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="9" t="s">
-        <v>123</v>
+        <v>299</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="9" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="9" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="9" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="9" t="s">
-        <v>127</v>
+        <v>300</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>150</v>
+        <v>68</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>138</v>
+      <c r="A68" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>149</v>
+      <c r="A69" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>139</v>
+      <c r="A70" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>146</v>
+        <v>273</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="9" t="s">
-        <v>120</v>
+        <v>301</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>145</v>
+        <v>72</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="9" t="s">
-        <v>119</v>
+      <c r="A73" s="8" t="s">
+        <v>302</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>144</v>
+        <v>303</v>
       </c>
       <c r="C73"/>
       <c r="F73" s="6"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="9" t="s">
-        <v>110</v>
+        <v>304</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>140</v>
+        <v>71</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>75</v>
+      <c r="A75" s="9" t="s">
+        <v>305</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" s="9" t="s">
-        <v>266</v>
-      </c>
-      <c r="B76" s="8" t="s">
-        <v>267</v>
+      <c r="A76" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="9" t="s">
-        <v>269</v>
-      </c>
-      <c r="B77" s="9" t="s">
-        <v>270</v>
+        <v>104</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="9" t="s">
-        <v>271</v>
-      </c>
-      <c r="B78" s="9" t="s">
-        <v>272</v>
+        <v>116</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="9" t="s">
-        <v>335</v>
-      </c>
-      <c r="B79" s="9" t="s">
-        <v>268</v>
+        <v>123</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="9" t="s">
-        <v>279</v>
-      </c>
-      <c r="B80" s="9" t="s">
-        <v>280</v>
+        <v>117</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="9" t="s">
-        <v>281</v>
-      </c>
-      <c r="B81" s="9" t="s">
-        <v>282</v>
+        <v>115</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>89</v>
+      <c r="A82" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>90</v>
+      <c r="A83" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="9" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="9" t="s">
-        <v>306</v>
+        <v>126</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="30" x14ac:dyDescent="0.2">
-      <c r="A86" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>240</v>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>77</v>
+      <c r="A87" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="9" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>237</v>
+      <c r="A89" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>91</v>
+      <c r="A90" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>223</v>
+      <c r="A91" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>78</v>
+      <c r="A92" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="B92" s="8" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>79</v>
+      <c r="A93" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="B93" s="9" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A94" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>80</v>
+      <c r="A94" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="B94" s="9" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>153</v>
+        <v>271</v>
+      </c>
+      <c r="B95" s="9" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A96" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>81</v>
+      <c r="A96" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="B96" s="9" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A97" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>82</v>
+      <c r="A97" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="B97" s="9" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="9" t="s">
-        <v>128</v>
+        <v>359</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>156</v>
+        <v>379</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A99" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="B99" s="9" t="s">
-        <v>155</v>
+      <c r="A99" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>154</v>
+      <c r="A100" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A101" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>83</v>
+      <c r="A101" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="B101" s="9" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="9" t="s">
-        <v>307</v>
+        <v>118</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>84</v>
+        <v>151</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="B103" s="9" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A104" s="9" t="s">
-        <v>308</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>85</v>
+        <v>306</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+      <c r="A104" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A105" s="9" t="s">
-        <v>293</v>
-      </c>
-      <c r="B105" s="9" t="s">
-        <v>292</v>
+      <c r="A105" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="9" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>92</v>
+        <v>237</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>93</v>
+        <v>15</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A109" s="3" t="s">
-        <v>40</v>
+      <c r="A109" s="7" t="s">
+        <v>225</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>95</v>
+        <v>223</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>94</v>
+        <v>31</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A111" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>96</v>
+      <c r="A111" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="B111" s="18" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="B112" s="9" t="s">
-        <v>158</v>
+      <c r="A112" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A113" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>86</v>
+      <c r="A113" s="18" t="s">
+        <v>329</v>
+      </c>
+      <c r="B113" s="18" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A114" s="7" t="s">
-        <v>294</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>222</v>
+      <c r="A114" s="18" t="s">
+        <v>331</v>
+      </c>
+      <c r="B114" s="18" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A115" s="7" t="s">
-        <v>257</v>
-      </c>
-      <c r="B115" s="7" t="s">
-        <v>258</v>
+      <c r="A115" s="18" t="s">
+        <v>316</v>
+      </c>
+      <c r="B115" s="18" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="18" t="s">
-        <v>247</v>
+        <v>314</v>
       </c>
       <c r="B116" s="18" t="s">
-        <v>246</v>
+        <v>315</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" s="18" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B117" s="18" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" s="18" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="B118" s="18" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" s="18" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="B119" s="18" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" s="18" t="s">
-        <v>316</v>
+        <v>333</v>
       </c>
       <c r="B120" s="18" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" s="18" t="s">
-        <v>318</v>
+        <v>327</v>
       </c>
       <c r="B121" s="18" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" s="18" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B122" s="18" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" s="18" t="s">
-        <v>322</v>
+        <v>336</v>
       </c>
       <c r="B123" s="18" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
@@ -3335,227 +3335,227 @@
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A125" s="18" t="s">
-        <v>336</v>
-      </c>
-      <c r="B125" s="18" t="s">
-        <v>326</v>
+      <c r="A125" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="B125" s="9" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A126" s="18" t="s">
-        <v>327</v>
-      </c>
-      <c r="B126" s="18" t="s">
-        <v>328</v>
+      <c r="A126" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="B126" s="9" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A127" s="18" t="s">
-        <v>329</v>
-      </c>
-      <c r="B127" s="18" t="s">
-        <v>330</v>
+      <c r="A127" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="B127" s="9" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A128" s="18" t="s">
-        <v>331</v>
-      </c>
-      <c r="B128" s="18" t="s">
-        <v>332</v>
+      <c r="A128" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="B128" s="9" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A129" s="18" t="s">
-        <v>333</v>
-      </c>
-      <c r="B129" s="18" t="s">
-        <v>334</v>
+      <c r="A129" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="B129" s="9" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A130" s="9" t="s">
-        <v>347</v>
-      </c>
-      <c r="B130" s="9" t="s">
-        <v>367</v>
+      <c r="A130" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" s="9" t="s">
-        <v>348</v>
-      </c>
-      <c r="B131" s="9" t="s">
-        <v>368</v>
+        <v>107</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A132" s="9" t="s">
-        <v>349</v>
-      </c>
-      <c r="B132" s="9" t="s">
-        <v>369</v>
+      <c r="A132" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A133" s="9" t="s">
-        <v>350</v>
-      </c>
-      <c r="B133" s="9" t="s">
-        <v>370</v>
+      <c r="A133" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" s="9" t="s">
-        <v>351</v>
+        <v>128</v>
       </c>
       <c r="B134" s="9" t="s">
-        <v>371</v>
+        <v>156</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" s="9" t="s">
-        <v>352</v>
+        <v>113</v>
       </c>
       <c r="B135" s="9" t="s">
-        <v>372</v>
+        <v>155</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" s="9" t="s">
-        <v>353</v>
-      </c>
-      <c r="B136" s="9" t="s">
-        <v>373</v>
+        <v>112</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A137" s="9" t="s">
-        <v>354</v>
-      </c>
-      <c r="B137" s="9" t="s">
-        <v>374</v>
+      <c r="A137" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" s="9" t="s">
-        <v>355</v>
-      </c>
-      <c r="B138" s="9" t="s">
-        <v>375</v>
+        <v>307</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" s="9" t="s">
-        <v>356</v>
+        <v>275</v>
       </c>
       <c r="B139" s="9" t="s">
-        <v>376</v>
+        <v>276</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" s="9" t="s">
-        <v>357</v>
-      </c>
-      <c r="B140" s="9" t="s">
-        <v>377</v>
+        <v>308</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" s="9" t="s">
-        <v>358</v>
+        <v>293</v>
       </c>
       <c r="B141" s="9" t="s">
-        <v>378</v>
+        <v>292</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" s="9" t="s">
-        <v>359</v>
-      </c>
-      <c r="B142" s="9" t="s">
-        <v>379</v>
+        <v>100</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A143" s="9" t="s">
-        <v>360</v>
-      </c>
-      <c r="B143" s="9" t="s">
-        <v>380</v>
+      <c r="A143" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A144" s="9" t="s">
-        <v>361</v>
-      </c>
-      <c r="B144" s="9" t="s">
-        <v>381</v>
+      <c r="A144" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A145" s="9" t="s">
-        <v>362</v>
-      </c>
-      <c r="B145" s="9" t="s">
-        <v>382</v>
+      <c r="A145" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A146" s="9" t="s">
-        <v>345</v>
-      </c>
-      <c r="B146" s="9" t="s">
-        <v>337</v>
+      <c r="A146" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A147" s="9" t="s">
-        <v>346</v>
-      </c>
-      <c r="B147" s="9" t="s">
-        <v>338</v>
+      <c r="A147" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" s="9" t="s">
-        <v>363</v>
+        <v>217</v>
       </c>
       <c r="B148" s="9" t="s">
-        <v>339</v>
+        <v>158</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A149" s="9" t="s">
-        <v>340</v>
-      </c>
-      <c r="B149" s="9" t="s">
-        <v>341</v>
+      <c r="A149" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A150" s="9" t="s">
-        <v>364</v>
-      </c>
-      <c r="B150" s="9" t="s">
-        <v>342</v>
+      <c r="A150" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A151" s="9" t="s">
-        <v>365</v>
-      </c>
-      <c r="B151" s="9" t="s">
-        <v>343</v>
+      <c r="A151" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="B151" s="7" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A152" s="9" t="s">
-        <v>366</v>
-      </c>
-      <c r="B152" s="9" t="s">
-        <v>344</v>
+      <c r="A152" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="B152" s="18" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
@@ -3564,7 +3564,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B129"/>
+  <autoFilter ref="A1:B129">
+    <sortState ref="A2:B152">
+      <sortCondition ref="A1:A152"/>
+    </sortState>
+  </autoFilter>
   <sortState ref="A2:B101">
     <sortCondition ref="A2:A101"/>
   </sortState>
@@ -3577,8 +3581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B121" sqref="B121"/>
     </sheetView>
   </sheetViews>
@@ -3777,51 +3781,51 @@
     </row>
     <row r="19" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="D19"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B20" s="9" t="s">
         <v>242</v>
-      </c>
-      <c r="D19"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>256</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>57</v>
+      <c r="A21" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>256</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>238</v>
+      <c r="A22" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="9" t="s">
-        <v>166</v>
+      <c r="A23" s="3" t="s">
+        <v>239</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>167</v>
+        <v>238</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
@@ -3829,10 +3833,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>178</v>
+        <v>166</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>167</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -3840,10 +3844,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>59</v>
+        <v>178</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
@@ -3851,10 +3855,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>162</v>
+        <v>59</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
@@ -3862,10 +3866,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>200</v>
+        <v>173</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>260</v>
+        <v>162</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
@@ -3873,10 +3877,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
@@ -3884,10 +3888,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
-        <v>171</v>
+        <v>199</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>220</v>
+        <v>261</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
@@ -3895,10 +3899,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>8</v>
+        <v>171</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>60</v>
+        <v>220</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
@@ -3906,10 +3910,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>179</v>
+        <v>8</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
@@ -3917,30 +3921,30 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>0</v>
+        <v>179</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
-        <v>277</v>
+        <v>0</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>278</v>
+        <v>62</v>
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
-        <v>161</v>
+        <v>277</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>181</v>
+        <v>278</v>
       </c>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
@@ -3948,10 +3952,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
-        <v>216</v>
+        <v>161</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>63</v>
+        <v>181</v>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
@@ -3959,10 +3963,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
-        <v>287</v>
+        <v>216</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>288</v>
+        <v>63</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
@@ -3970,10 +3974,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
@@ -3981,10 +3985,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>262</v>
+        <v>289</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>290</v>
       </c>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
@@ -3992,10 +3996,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>64</v>
+        <v>201</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>262</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
@@ -4003,10 +4007,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
-        <v>172</v>
+        <v>7</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>218</v>
+        <v>64</v>
       </c>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
@@ -4014,60 +4018,60 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>222</v>
+        <v>172</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>218</v>
       </c>
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>65</v>
+        <v>182</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>222</v>
       </c>
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
-        <v>283</v>
+        <v>170</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>284</v>
+        <v>66</v>
       </c>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
-        <v>169</v>
+        <v>283</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>67</v>
+        <v>284</v>
       </c>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
-        <v>124</v>
+        <v>169</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>133</v>
+        <v>67</v>
       </c>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
@@ -4075,665 +4079,665 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
-        <v>208</v>
+        <v>111</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>68</v>
+        <v>135</v>
       </c>
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
-        <v>160</v>
+        <v>208</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>163</v>
+        <v>68</v>
       </c>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>136</v>
+        <v>163</v>
       </c>
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E52" s="6"/>
       <c r="F52" s="6"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
-        <v>273</v>
+        <v>101</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>274</v>
+        <v>132</v>
       </c>
       <c r="F53" s="6"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="9" t="s">
-        <v>202</v>
+        <v>273</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>69</v>
+        <v>274</v>
       </c>
       <c r="F54" s="6"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F55" s="6"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F56" s="6"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="9" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F57" s="6"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="9" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F58" s="6"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F59" s="6"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="9" t="s">
-        <v>104</v>
+        <v>206</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>137</v>
+        <v>74</v>
       </c>
       <c r="F60" s="6"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="9" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F61" s="6"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="9" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="F62" s="6"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="9" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="F63" s="6"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="9" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="F64" s="6"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="9" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="F65" s="6"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="9" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F66" s="6"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="9" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="F67" s="6"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="9" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="F68" s="6"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="9" t="s">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="F69" s="6"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="9" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D70" s="6"/>
       <c r="F70" s="6"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F71" s="6"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="9" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F72" s="6"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="9" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D73" s="6"/>
       <c r="F73" s="6"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="9" t="s">
-        <v>266</v>
-      </c>
-      <c r="B74" s="8" t="s">
-        <v>267</v>
+        <v>110</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>140</v>
       </c>
       <c r="D74" s="6"/>
       <c r="F74" s="6"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="9" t="s">
-        <v>269</v>
-      </c>
-      <c r="B75" s="9" t="s">
-        <v>270</v>
+        <v>266</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>267</v>
       </c>
       <c r="D75" s="6"/>
       <c r="F75" s="6"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="9" t="s">
-        <v>271</v>
+        <v>335</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="F76" s="6"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="9" t="s">
-        <v>335</v>
+        <v>269</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="F77" s="6"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="9" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="D78" s="6"/>
       <c r="F78" s="6"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="9" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D79" s="6"/>
       <c r="F79" s="6"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="9" t="s">
-        <v>209</v>
+        <v>281</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>75</v>
+        <v>282</v>
       </c>
       <c r="F80" s="6"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="9" t="s">
-        <v>118</v>
+        <v>209</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>151</v>
+        <v>75</v>
       </c>
       <c r="D81" s="6"/>
       <c r="F81" s="6"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="9" t="s">
-        <v>194</v>
+        <v>118</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>76</v>
+        <v>151</v>
       </c>
       <c r="D82" s="6"/>
       <c r="F82" s="6"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="9" t="s">
-        <v>103</v>
+        <v>194</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>152</v>
+        <v>76</v>
       </c>
       <c r="F83" s="6"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="9" t="s">
-        <v>210</v>
+        <v>103</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>77</v>
+        <v>152</v>
       </c>
       <c r="F84" s="6"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="9" t="s">
-        <v>18</v>
+        <v>210</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>237</v>
+        <v>77</v>
       </c>
       <c r="F85" s="6"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="9" t="s">
-        <v>189</v>
+        <v>18</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>164</v>
+        <v>237</v>
       </c>
       <c r="F86" s="6"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="9" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F87" s="6"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="9" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>78</v>
+        <v>165</v>
       </c>
       <c r="F88" s="6"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="B89" s="9" t="s">
-        <v>79</v>
+      <c r="A89" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="B89" s="18" t="s">
+        <v>311</v>
       </c>
       <c r="F89" s="6"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="9" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>175</v>
+        <v>78</v>
       </c>
       <c r="F90" s="6"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="9" t="s">
-        <v>176</v>
+        <v>213</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D91" s="6"/>
       <c r="F91" s="6"/>
     </row>
     <row r="92" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="B92" s="9" t="s">
-        <v>153</v>
+      <c r="A92" s="18" t="s">
+        <v>329</v>
+      </c>
+      <c r="B92" s="18" t="s">
+        <v>330</v>
       </c>
       <c r="D92"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A93" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B93" s="9" t="s">
-        <v>81</v>
+      <c r="A93" s="18" t="s">
+        <v>331</v>
+      </c>
+      <c r="B93" s="18" t="s">
+        <v>332</v>
       </c>
       <c r="D93" s="6"/>
       <c r="F93" s="6"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A94" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B94" s="9" t="s">
-        <v>82</v>
+      <c r="A94" s="18" t="s">
+        <v>316</v>
+      </c>
+      <c r="B94" s="18" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A95" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="B95" s="9" t="s">
-        <v>156</v>
+      <c r="A95" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="B95" s="18" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A96" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="B96" s="9" t="s">
-        <v>155</v>
+      <c r="A96" s="18" t="s">
+        <v>312</v>
+      </c>
+      <c r="B96" s="18" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A97" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="B97" s="9" t="s">
-        <v>154</v>
+      <c r="A97" s="18" t="s">
+        <v>318</v>
+      </c>
+      <c r="B97" s="18" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A98" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="B98" s="9" t="s">
-        <v>276</v>
+      <c r="A98" s="18" t="s">
+        <v>320</v>
+      </c>
+      <c r="B98" s="18" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A99" s="9" t="s">
-        <v>293</v>
-      </c>
-      <c r="B99" s="9" t="s">
-        <v>292</v>
+      <c r="A99" s="18" t="s">
+        <v>333</v>
+      </c>
+      <c r="B99" s="18" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="B100" s="9" t="s">
-        <v>157</v>
+      <c r="A100" s="18" t="s">
+        <v>327</v>
+      </c>
+      <c r="B100" s="18" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A101" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="B101" s="9" t="s">
-        <v>158</v>
+      <c r="A101" s="18" t="s">
+        <v>322</v>
+      </c>
+      <c r="B101" s="18" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A102" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="B102" s="9" t="s">
-        <v>83</v>
+      <c r="A102" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="B102" s="18" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A103" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="B103" s="9" t="s">
-        <v>84</v>
+      <c r="A103" s="18" t="s">
+        <v>324</v>
+      </c>
+      <c r="B103" s="18" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="9" t="s">
-        <v>214</v>
+        <v>174</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>85</v>
+        <v>175</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B105" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B106" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B107" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B108" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B109" s="9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B110" s="9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B111" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="B112" s="9" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="B113" s="9" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B114" s="9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="B115" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="B116" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="B117" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="B118" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B105" s="9" t="s">
+      <c r="B119" s="9" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A106" s="7" t="s">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="B106" s="7" t="s">
+      <c r="B120" s="7" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A107" s="22" t="s">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" s="22" t="s">
         <v>247</v>
       </c>
-      <c r="B107" s="22" t="s">
+      <c r="B121" s="22" t="s">
         <v>246</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A108" s="18" t="s">
-        <v>310</v>
-      </c>
-      <c r="B108" s="18" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A109" s="18" t="s">
-        <v>312</v>
-      </c>
-      <c r="B109" s="18" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A110" s="18" t="s">
-        <v>314</v>
-      </c>
-      <c r="B110" s="18" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A111" s="18" t="s">
-        <v>316</v>
-      </c>
-      <c r="B111" s="18" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" s="18" t="s">
-        <v>318</v>
-      </c>
-      <c r="B112" s="18" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A113" s="18" t="s">
-        <v>320</v>
-      </c>
-      <c r="B113" s="18" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A114" s="18" t="s">
-        <v>322</v>
-      </c>
-      <c r="B114" s="18" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A115" s="18" t="s">
-        <v>324</v>
-      </c>
-      <c r="B115" s="18" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A116" s="18" t="s">
-        <v>336</v>
-      </c>
-      <c r="B116" s="18" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A117" s="18" t="s">
-        <v>327</v>
-      </c>
-      <c r="B117" s="18" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A118" s="18" t="s">
-        <v>329</v>
-      </c>
-      <c r="B118" s="18" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A119" s="18" t="s">
-        <v>331</v>
-      </c>
-      <c r="B119" s="18" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A120" s="18" t="s">
-        <v>333</v>
-      </c>
-      <c r="B120" s="18" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A121" s="9" t="s">
-        <v>362</v>
-      </c>
-      <c r="B121" s="9" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
@@ -4743,8 +4747,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:B89">
-    <sortState ref="A2:B107">
-      <sortCondition ref="A1:A107"/>
+    <sortState ref="A2:B121">
+      <sortCondition ref="A1:A121"/>
     </sortState>
   </autoFilter>
   <sortState ref="D2:D93">

</xml_diff>